<commit_message>
[MODIFY] results and script for simulation of metabolites in sp for multi quercus model
</commit_message>
<xml_diff>
--- a/validation/quercus/simulation_sp/produced_at_day_multi_quercus.xlsx
+++ b/validation/quercus/simulation_sp/produced_at_day_multi_quercus.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,17 +458,17 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Sucrose__Leaf_Day_sp_exchange</t>
+          <t>Sucrose__Ibark_Day_sp_exchange</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5.215439237065897e-05</v>
+        <v>0.01195219123505989</v>
       </c>
       <c r="C2" t="n">
-        <v>-41.28124359522034</v>
+        <v>-41.26647142419872</v>
       </c>
       <c r="D2" t="n">
-        <v>50.53486493485336</v>
+        <v>41.26647142419873</v>
       </c>
       <c r="E2" t="b">
         <v>0</v>
@@ -477,17 +477,17 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Sucrose__Ibark_Day_sp_exchange</t>
+          <t>L-Proline__Leaf_Day_sp_exchange</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.01211188350113235</v>
+        <v>0.15</v>
       </c>
       <c r="C3" t="n">
-        <v>-41.2437747925777</v>
+        <v>-21.32001438946436</v>
       </c>
       <c r="D3" t="n">
-        <v>41.24359042609948</v>
+        <v>25.78744231144447</v>
       </c>
       <c r="E3" t="b">
         <v>0</v>
@@ -496,17 +496,17 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>L-Leucine__Leaf_Day_sp_exchange</t>
+          <t>L-Proline__Phellogen_Day_sp_exchange</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>6.258925787692502e-06</v>
+        <v>0.02777777777777782</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.06201957726875846</v>
+        <v>-12.53780877226151</v>
       </c>
       <c r="D4" t="n">
-        <v>0.06041820219998738</v>
+        <v>12.56905456040514</v>
       </c>
       <c r="E4" t="b">
         <v>0</v>
@@ -515,171 +515,19 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>L-Threonine__Ibark_Day_sp_exchange</t>
+          <t>Citrate__Phellogen_Day_sp_exchange</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2.168512424198476e-05</v>
+        <v>0.02777777777777785</v>
       </c>
       <c r="C5" t="n">
-        <v>-11.22246289176266</v>
+        <v>-7.268536966848401</v>
       </c>
       <c r="D5" t="n">
-        <v>10.96557426871229</v>
+        <v>7.276804028092124</v>
       </c>
       <c r="E5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>L-Threonine__Phellogen_Day_sp_exchange</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>1.416469826012178e-05</v>
-      </c>
-      <c r="C6" t="n">
-        <v>-10.63828984401221</v>
-      </c>
-      <c r="D6" t="n">
-        <v>10.22552626201239</v>
-      </c>
-      <c r="E6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>L-Proline__Leaf_Day_sp_exchange</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>0.1501444482061617</v>
-      </c>
-      <c r="C7" t="n">
-        <v>-21.31005312688049</v>
-      </c>
-      <c r="D7" t="n">
-        <v>25.77512175686455</v>
-      </c>
-      <c r="E7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>L-Proline__Phellogen_Day_sp_exchange</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>0.02773499615518548</v>
-      </c>
-      <c r="C8" t="n">
-        <v>-12.53135495996923</v>
-      </c>
-      <c r="D8" t="n">
-        <v>12.56264708872167</v>
-      </c>
-      <c r="E8" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="inlineStr">
-        <is>
-          <t>L-Serine__Leaf_Day_sp_exchange</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>1.043633051810705e-05</v>
-      </c>
-      <c r="C9" t="n">
-        <v>-6.398536363892759</v>
-      </c>
-      <c r="D9" t="n">
-        <v>6.522138555141318</v>
-      </c>
-      <c r="E9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="inlineStr">
-        <is>
-          <t>L-Serine__Ibark_Day_sp_exchange</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>7.056672741985366e-05</v>
-      </c>
-      <c r="C10" t="n">
-        <v>-6.315139342797044</v>
-      </c>
-      <c r="D10" t="n">
-        <v>6.306203923756939</v>
-      </c>
-      <c r="E10" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="inlineStr">
-        <is>
-          <t>L-Serine__Phellogen_Day_sp_exchange</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>9.041351003363021e-06</v>
-      </c>
-      <c r="C11" t="n">
-        <v>-5.7277184959369</v>
-      </c>
-      <c r="D11" t="n">
-        <v>5.737683763999101</v>
-      </c>
-      <c r="E11" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="inlineStr">
-        <is>
-          <t>Fumarate__Leaf_Day_sp_exchange</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>1.660663567033179e-05</v>
-      </c>
-      <c r="C12" t="n">
-        <v>-50.47564632122968</v>
-      </c>
-      <c r="D12" t="n">
-        <v>43.18074302902186</v>
-      </c>
-      <c r="E12" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="inlineStr">
-        <is>
-          <t>Citrate__Phellogen_Day_sp_exchange</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>0.02766042752066101</v>
-      </c>
-      <c r="C13" t="n">
-        <v>-7.265607050869296</v>
-      </c>
-      <c r="D13" t="n">
-        <v>7.273880518447664</v>
-      </c>
-      <c r="E13" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[ADD] QY&AQ for tomato 2015 model + [MODIFY] minor changes on test_dfa_multiquercus.py, simulation_sp_multi_quercus.py, QY-Maize_Saha.py and quercus_reactions_fluxes.py files
</commit_message>
<xml_diff>
--- a/validation/quercus/simulation_sp/produced_at_day_multi_quercus.xlsx
+++ b/validation/quercus/simulation_sp/produced_at_day_multi_quercus.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,36 +458,36 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Sucrose__Ibark_Day_sp_exchange</t>
+          <t>Sucrose__Leaf_Day_sp_exchange</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.01195219123505989</v>
+        <v>0.1687925060738079</v>
       </c>
       <c r="C2" t="n">
-        <v>-41.26647142419872</v>
+        <v>0.06406739917233768</v>
       </c>
       <c r="D2" t="n">
-        <v>41.26647142419873</v>
+        <v>0.6903782242560664</v>
       </c>
       <c r="E2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>L-Proline__Leaf_Day_sp_exchange</t>
+          <t>Sucrose__Ibark_Day_sp_exchange</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.15</v>
+        <v>0.2406323589257673</v>
       </c>
       <c r="C3" t="n">
-        <v>-21.32001438946436</v>
+        <v>-0.5216777508955427</v>
       </c>
       <c r="D3" t="n">
-        <v>25.78744231144447</v>
+        <v>0.4141614131960218</v>
       </c>
       <c r="E3" t="b">
         <v>0</v>
@@ -496,38 +496,532 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>L-Proline__Phellogen_Day_sp_exchange</t>
+          <t>Sulfate__Leaf_Day_sp_exchange</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.02777777777777782</v>
+        <v>0.003504055077490749</v>
       </c>
       <c r="C4" t="n">
-        <v>-12.53780877226151</v>
+        <v>0.002060902692307016</v>
       </c>
       <c r="D4" t="n">
-        <v>12.56905456040514</v>
+        <v>0.003505050408745101</v>
       </c>
       <c r="E4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Citrate__Phellogen_Day_sp_exchange</t>
+          <t>Sulfate__Phellogen_Day_sp_exchange</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.02777777777777785</v>
+        <v>2.22852643092e-05</v>
       </c>
       <c r="C5" t="n">
-        <v>-7.268536966848401</v>
+        <v>-0.0001784322011307188</v>
       </c>
       <c r="D5" t="n">
-        <v>7.276804028092124</v>
+        <v>2.394769507019581e-05</v>
       </c>
       <c r="E5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>L-Histidine__Leaf_Day_sp_exchange</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.00343914788412</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.003384834976915411</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.006322199359902263</v>
+      </c>
+      <c r="E6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>L-Histidine__Ibark_Day_sp_exchange</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.001134476891184</v>
+      </c>
+      <c r="C7" t="n">
+        <v>-0.001747949722832976</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.001747941670666604</v>
+      </c>
+      <c r="E7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>L-Histidine__Phellogen_Day_sp_exchange</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.000306732348</v>
+      </c>
+      <c r="C8" t="n">
+        <v>-0.0003067364158244874</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.0003067323897413055</v>
+      </c>
+      <c r="E8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>L-Isoleucine__Leaf_Day_sp_exchange</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.006721185196974926</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.00661204631838521</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.0123561532909376</v>
+      </c>
+      <c r="E9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>L-Isoleucine__Ibark_Day_sp_exchange</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.002217127481273602</v>
+      </c>
+      <c r="C10" t="n">
+        <v>-0.003416548011990307</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.003416532201130997</v>
+      </c>
+      <c r="E10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>L-Isoleucine__Phellogen_Day_sp_exchange</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0.000599539998</v>
+      </c>
+      <c r="C11" t="n">
+        <v>-0.0005995479823031534</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.0005995400795876852</v>
+      </c>
+      <c r="E11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>L-Methionine__Leaf_Day_sp_exchange</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0.003194694700287325</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.003192232806831969</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.005872215524106884</v>
+      </c>
+      <c r="E12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>L-Methionine__Ibark_Day_sp_exchange</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0.001053832118206579</v>
+      </c>
+      <c r="C13" t="n">
+        <v>-0.001623696085067752</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.001623688415129498</v>
+      </c>
+      <c r="E13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>L-Methionine__Phellogen_Day_sp_exchange</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0.0002849281484882077</v>
+      </c>
+      <c r="C14" t="n">
+        <v>-0.0002849281500259943</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.0002849281484881792</v>
+      </c>
+      <c r="E14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>L-Threonine__Ibark_Day_sp_exchange</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.04329293223488179</v>
+      </c>
+      <c r="C15" t="n">
+        <v>-0.04454761266755076</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.04454305664664826</v>
+      </c>
+      <c r="E15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>L-Threonine__Phellogen_Day_sp_exchange</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0.000624934156475544</v>
+      </c>
+      <c r="C16" t="n">
+        <v>-0.0006291993058224769</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.0006258866057571672</v>
+      </c>
+      <c r="E16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>L-Arginine__Leaf_Day_sp_exchange</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>0.008007488108685002</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.008005499327275109</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.01472542850905506</v>
+      </c>
+      <c r="E17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>L-Arginine__Ibark_Day_sp_exchange</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>0.002641442160042</v>
+      </c>
+      <c r="C18" t="n">
+        <v>-0.004105226759005759</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.004071540413824702</v>
+      </c>
+      <c r="E18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>L-Arginine__Phellogen_Day_sp_exchange</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>0.0007141756364999999</v>
+      </c>
+      <c r="C19" t="n">
+        <v>-0.0007225215059462023</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.0007161534346236177</v>
+      </c>
+      <c r="E19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>Glycine__Leaf_Day_sp_exchange</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>0.5554246233815529</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.5554218912339979</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.5554247109920823</v>
+      </c>
+      <c r="E20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>L-Proline__Leaf_Day_sp_exchange</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>0.2402842689810597</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.2328272519035937</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.2903230428217639</v>
+      </c>
+      <c r="E21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>L-Proline__Ibark_Day_sp_exchange</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>0.002229608120362</v>
+      </c>
+      <c r="C22" t="n">
+        <v>-0.05312921603794164</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.04788798295784884</v>
+      </c>
+      <c r="E22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>L-Proline__Phellogen_Day_sp_exchange</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>0.009753234929701014</v>
+      </c>
+      <c r="C23" t="n">
+        <v>-0.05029678126141199</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.04505554815223743</v>
+      </c>
+      <c r="E23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>L-Tyrosine__Leaf_Day_sp_exchange</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>0.003653762406255001</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0.003653301279022389</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.00671621885767548</v>
+      </c>
+      <c r="E24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>L-Tyrosine__Ibark_Day_sp_exchange</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>0.001205272106766</v>
+      </c>
+      <c r="C25" t="n">
+        <v>-0.001857437265177838</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0.001857184344654449</v>
+      </c>
+      <c r="E25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>L-Tyrosine__Phellogen_Day_sp_exchange</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>0.0003258734895</v>
+      </c>
+      <c r="C26" t="n">
+        <v>-0.0003262916688125919</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0.0003260387483883785</v>
+      </c>
+      <c r="E26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="inlineStr">
+        <is>
+          <t>L-Glutamate__Ibark_Day_sp_exchange</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>0.01800172555858616</v>
+      </c>
+      <c r="C27" t="n">
+        <v>-0.07424956162034638</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.09091255874618542</v>
+      </c>
+      <c r="E27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t>beta-D-Fructose__Ibark_Day_sp_exchange</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>0.1228081432742556</v>
+      </c>
+      <c r="C28" t="n">
+        <v>-0.2910826847497351</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0.6368100207591254</v>
+      </c>
+      <c r="E28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>beta-D-Fructose__Phellogen_Day_sp_exchange</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>0.02275250248137701</v>
+      </c>
+      <c r="C29" t="n">
+        <v>-0.02526205466183172</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0.0257352701600722</v>
+      </c>
+      <c r="E29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="inlineStr">
+        <is>
+          <t>Fumarate__Leaf_Day_sp_exchange</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>0.1494590463445943</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0.1489928864234148</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.1549827317848688</v>
+      </c>
+      <c r="E30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="inlineStr">
+        <is>
+          <t>Fumarate__Phellogen_Day_sp_exchange</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>0.03724699327866923</v>
+      </c>
+      <c r="C31" t="n">
+        <v>-0.06148366282853604</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0.1669730896936179</v>
+      </c>
+      <c r="E31" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[FIX] fixation of biomass reaction flux at 0.11
</commit_message>
<xml_diff>
--- a/validation/quercus/simulation_sp/produced_at_day_multi_quercus.xlsx
+++ b/validation/quercus/simulation_sp/produced_at_day_multi_quercus.xlsx
@@ -462,13 +462,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.1687925060738079</v>
+        <v>0.1856717566753563</v>
       </c>
       <c r="C2" t="n">
-        <v>0.06406739917233768</v>
+        <v>0.07047413908644458</v>
       </c>
       <c r="D2" t="n">
-        <v>0.6903782242560664</v>
+        <v>0.7680937323029654</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
@@ -481,13 +481,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2406323589257673</v>
+        <v>0.2619045040918823</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.5216777508955427</v>
+        <v>-0.5570318527331276</v>
       </c>
       <c r="D3" t="n">
-        <v>0.4141614131960218</v>
+        <v>0.4406610716981233</v>
       </c>
       <c r="E3" t="b">
         <v>0</v>
@@ -500,13 +500,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.003504055077490749</v>
+        <v>0.00385446058523984</v>
       </c>
       <c r="C4" t="n">
-        <v>0.002060902692307016</v>
+        <v>0.003744014416556215</v>
       </c>
       <c r="D4" t="n">
-        <v>0.003505050408745101</v>
+        <v>0.003856417738732076</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
@@ -519,13 +519,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2.22852643092e-05</v>
+        <v>2.451379074012e-05</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.0001784322011307188</v>
+        <v>-3.748731746025131e-05</v>
       </c>
       <c r="D5" t="n">
-        <v>2.394769507019581e-05</v>
+        <v>2.769017620040231e-05</v>
       </c>
       <c r="E5" t="b">
         <v>0</v>
@@ -538,13 +538,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.00343914788412</v>
+        <v>0.003783062672532</v>
       </c>
       <c r="C6" t="n">
-        <v>0.003384834976915411</v>
+        <v>0.003778713351258491</v>
       </c>
       <c r="D6" t="n">
-        <v>0.006322199359902263</v>
+        <v>0.006953723701989898</v>
       </c>
       <c r="E6" t="b">
         <v>1</v>
@@ -557,13 +557,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.001134476891184</v>
+        <v>0.0012479245803024</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.001747949722832976</v>
+        <v>-0.001922736397396834</v>
       </c>
       <c r="D7" t="n">
-        <v>0.001747941670666604</v>
+        <v>0.00192273590541154</v>
       </c>
       <c r="E7" t="b">
         <v>0</v>
@@ -576,13 +576,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.000306732348</v>
+        <v>0.0003374055828</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.0003067364158244874</v>
+        <v>-0.0003374059085472175</v>
       </c>
       <c r="D8" t="n">
-        <v>0.0003067323897413055</v>
+        <v>0.0003374056625545708</v>
       </c>
       <c r="E8" t="b">
         <v>0</v>
@@ -595,13 +595,13 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.006721185196974926</v>
+        <v>0.007393303716672417</v>
       </c>
       <c r="C9" t="n">
-        <v>0.00661204631838521</v>
+        <v>0.00738415862926447</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0123561532909376</v>
+        <v>0.01359176908201526</v>
       </c>
       <c r="E9" t="b">
         <v>1</v>
@@ -614,13 +614,13 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.002217127481273602</v>
+        <v>0.002438840229400962</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.003416548011990307</v>
+        <v>-0.003758186558964031</v>
       </c>
       <c r="D10" t="n">
-        <v>0.003416532201130997</v>
+        <v>0.003758185535317971</v>
       </c>
       <c r="E10" t="b">
         <v>0</v>
@@ -633,13 +633,13 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.000599539998</v>
+        <v>0.0006594939978</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.0005995479823031534</v>
+        <v>-0.0006594946534208139</v>
       </c>
       <c r="D11" t="n">
-        <v>0.0005995400795876852</v>
+        <v>0.0006594941536885299</v>
       </c>
       <c r="E11" t="b">
         <v>0</v>
@@ -652,13 +652,13 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.003194694700287325</v>
+        <v>0.003514164170316058</v>
       </c>
       <c r="C12" t="n">
-        <v>0.003192232806831969</v>
+        <v>0.00351036866946521</v>
       </c>
       <c r="D12" t="n">
-        <v>0.005872215524106884</v>
+        <v>0.006459437408770986</v>
       </c>
       <c r="E12" t="b">
         <v>1</v>
@@ -671,13 +671,13 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.001053832118206579</v>
+        <v>0.001159215330027195</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.001623696085067752</v>
+        <v>-0.001786057256931095</v>
       </c>
       <c r="D13" t="n">
-        <v>0.001623688415129498</v>
+        <v>0.001786057257079671</v>
       </c>
       <c r="E13" t="b">
         <v>0</v>
@@ -690,13 +690,13 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.0002849281484882077</v>
+        <v>0.000313420963337019</v>
       </c>
       <c r="C14" t="n">
-        <v>-0.0002849281500259943</v>
+        <v>-0.0003134209693209057</v>
       </c>
       <c r="D14" t="n">
-        <v>0.0002849281484881792</v>
+        <v>0.0003134209687925157</v>
       </c>
       <c r="E14" t="b">
         <v>0</v>
@@ -709,13 +709,13 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.04329293223488179</v>
+        <v>0.04762222545836997</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.04454761266755076</v>
+        <v>-0.04899668581452484</v>
       </c>
       <c r="D15" t="n">
-        <v>0.04454305664664826</v>
+        <v>0.04899763777056636</v>
       </c>
       <c r="E15" t="b">
         <v>0</v>
@@ -728,13 +728,13 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.000624934156475544</v>
+        <v>0.0006874275721230985</v>
       </c>
       <c r="C16" t="n">
-        <v>-0.0006291993058224769</v>
+        <v>-0.0006870891156657752</v>
       </c>
       <c r="D16" t="n">
-        <v>0.0006258866057571672</v>
+        <v>0.0006888209719004614</v>
       </c>
       <c r="E16" t="b">
         <v>0</v>
@@ -747,13 +747,13 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.008007488108685002</v>
+        <v>0.0088082369195535</v>
       </c>
       <c r="C17" t="n">
-        <v>0.008005499327275109</v>
+        <v>0.008808060179282796</v>
       </c>
       <c r="D17" t="n">
-        <v>0.01472542850905506</v>
+        <v>0.01620067687608405</v>
       </c>
       <c r="E17" t="b">
         <v>1</v>
@@ -766,13 +766,13 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.002641442160042</v>
+        <v>0.0029055863760462</v>
       </c>
       <c r="C18" t="n">
-        <v>-0.004105226759005759</v>
+        <v>-0.00450011261817293</v>
       </c>
       <c r="D18" t="n">
-        <v>0.004071540413824702</v>
+        <v>0.004479147180510654</v>
       </c>
       <c r="E18" t="b">
         <v>0</v>
@@ -785,13 +785,13 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.0007141756364999999</v>
+        <v>0.00078559320015</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.0007225215059462023</v>
+        <v>-0.0007905945278937255</v>
       </c>
       <c r="D19" t="n">
-        <v>0.0007161534346236177</v>
+        <v>0.0007867804015717369</v>
       </c>
       <c r="E19" t="b">
         <v>0</v>
@@ -804,13 +804,13 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.5554246233815529</v>
+        <v>0.6109670852943134</v>
       </c>
       <c r="C20" t="n">
-        <v>0.5554218912339979</v>
+        <v>0.6109642550659238</v>
       </c>
       <c r="D20" t="n">
-        <v>0.5554247109920823</v>
+        <v>0.6109670858853445</v>
       </c>
       <c r="E20" t="b">
         <v>1</v>
@@ -823,13 +823,13 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.2402842689810597</v>
+        <v>0.2493126962523645</v>
       </c>
       <c r="C21" t="n">
-        <v>0.2328272519035937</v>
+        <v>0.249153365156595</v>
       </c>
       <c r="D21" t="n">
-        <v>0.2903230428217639</v>
+        <v>0.3043093884402824</v>
       </c>
       <c r="E21" t="b">
         <v>1</v>
@@ -842,13 +842,13 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.002229608120362</v>
+        <v>0.0024525689323982</v>
       </c>
       <c r="C22" t="n">
-        <v>-0.05312921603794164</v>
+        <v>-0.05263003112399434</v>
       </c>
       <c r="D22" t="n">
-        <v>0.04788798295784884</v>
+        <v>0.05258133794884957</v>
       </c>
       <c r="E22" t="b">
         <v>0</v>
@@ -861,13 +861,13 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.009753234929701014</v>
+        <v>0.003304802308192157</v>
       </c>
       <c r="C23" t="n">
-        <v>-0.05029678126141199</v>
+        <v>-0.0495143528465315</v>
       </c>
       <c r="D23" t="n">
-        <v>0.04505554815223743</v>
+        <v>0.04946565967221674</v>
       </c>
       <c r="E23" t="b">
         <v>0</v>
@@ -880,13 +880,13 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.003653762406255001</v>
+        <v>0.004019138646880501</v>
       </c>
       <c r="C24" t="n">
-        <v>0.003653301279022389</v>
+        <v>0.004018556396839812</v>
       </c>
       <c r="D24" t="n">
-        <v>0.00671621885767548</v>
+        <v>0.007387748966675581</v>
       </c>
       <c r="E24" t="b">
         <v>1</v>
@@ -899,13 +899,13 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.001205272106766</v>
+        <v>0.0013257993174426</v>
       </c>
       <c r="C25" t="n">
-        <v>-0.001857437265177838</v>
+        <v>-0.002043204413876881</v>
       </c>
       <c r="D25" t="n">
-        <v>0.001857184344654449</v>
+        <v>0.002042811002352116</v>
       </c>
       <c r="E25" t="b">
         <v>0</v>
@@ -918,13 +918,13 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.0003258734895</v>
+        <v>0.00035846083845</v>
       </c>
       <c r="C26" t="n">
-        <v>-0.0003262916688125919</v>
+        <v>-0.0003589442579871089</v>
       </c>
       <c r="D26" t="n">
-        <v>0.0003260387483883785</v>
+        <v>0.0003585508464594493</v>
       </c>
       <c r="E26" t="b">
         <v>0</v>
@@ -937,13 +937,13 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.01800172555858616</v>
+        <v>0.01980189811444471</v>
       </c>
       <c r="C27" t="n">
-        <v>-0.07424956162034638</v>
+        <v>-0.07519053436097996</v>
       </c>
       <c r="D27" t="n">
-        <v>0.09091255874618542</v>
+        <v>0.09287352973702369</v>
       </c>
       <c r="E27" t="b">
         <v>0</v>
@@ -956,13 +956,13 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.1228081432742556</v>
+        <v>0.1355565840021052</v>
       </c>
       <c r="C28" t="n">
-        <v>-0.2910826847497351</v>
+        <v>-0.3015312766721112</v>
       </c>
       <c r="D28" t="n">
-        <v>0.6368100207591254</v>
+        <v>0.673569684293486</v>
       </c>
       <c r="E28" t="b">
         <v>0</v>
@@ -975,13 +975,13 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.02275250248137701</v>
+        <v>0.02371014509725695</v>
       </c>
       <c r="C29" t="n">
-        <v>-0.02526205466183172</v>
+        <v>-0.02565769299097373</v>
       </c>
       <c r="D29" t="n">
-        <v>0.0257352701600722</v>
+        <v>0.02798978154973403</v>
       </c>
       <c r="E29" t="b">
         <v>0</v>
@@ -994,13 +994,13 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.1494590463445943</v>
+        <v>0.1644049506903602</v>
       </c>
       <c r="C30" t="n">
-        <v>0.1489928864234148</v>
+        <v>0.1640875153414896</v>
       </c>
       <c r="D30" t="n">
-        <v>0.1549827317848688</v>
+        <v>0.1699549874337685</v>
       </c>
       <c r="E30" t="b">
         <v>1</v>
@@ -1013,13 +1013,13 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0.03724699327866923</v>
+        <v>0.04097169260652332</v>
       </c>
       <c r="C31" t="n">
-        <v>-0.06148366282853604</v>
+        <v>-0.06400639216058052</v>
       </c>
       <c r="D31" t="n">
-        <v>0.1669730896936179</v>
+        <v>0.1729259130713995</v>
       </c>
       <c r="E31" t="b">
         <v>0</v>

</xml_diff>